<commit_message>
Prepare and do 3^2 experiments
Changelog:
> Modify .gitignore to exclude .jpg, .docx
> Calibrate hematocrit and clean up Hematocrit directory
> Modify dimensionalize to calculate hematocrits
> Digitize spin profile into frames for experimental times
> Do 3^2 experiments (xlsx and RMD files mostly affected)
> Make velocity_functions more flexible
</commit_message>
<xml_diff>
--- a/Data-analysis/contact angles.xlsx
+++ b/Data-analysis/contact angles.xlsx
@@ -1,36 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\groups\bloodfilter\CliftonAnderson\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdhig\Documents\MS-Thesis-Pitt\Data-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81826F11-A53F-4957-9E60-F02FEE4A26CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16455" windowHeight="6105"/>
+    <workbookView xWindow="1884" yWindow="720" windowWidth="16548" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$P$196</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Clifton Anderson</author>
   </authors>
   <commentList>
-    <comment ref="B1" authorId="0" shapeId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -54,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -80,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H50" authorId="0" shapeId="0">
+    <comment ref="H50" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F126" authorId="0" shapeId="0">
+    <comment ref="F126" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +122,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Clifton Anderson:</t>
         </r>
@@ -121,7 +131,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 missing some matte data from this day
@@ -134,12 +144,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Clifton Anderson</author>
   </authors>
   <commentList>
-    <comment ref="L1" authorId="0" shapeId="0">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H50" authorId="0" shapeId="0">
+    <comment ref="H50" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -194,7 +204,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2734" uniqueCount="197">
   <si>
     <t>Drop</t>
   </si>
@@ -790,8 +800,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -811,19 +821,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -890,7 +887,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B6A8916F-B600-41B2-96C8-C9A99DEF6D61}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B6A8916F-B600-41B2-96C8-C9A99DEF6D61}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -934,7 +931,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DB97CF66-022D-401D-925F-22B0A61F7546}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB97CF66-022D-401D-925F-22B0A61F7546}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -963,14 +960,14 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>245404</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:colOff>350179</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>29</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -978,7 +975,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9724C010-4FCB-4FB1-BF51-A43E90F1BD98}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9724C010-4FCB-4FB1-BF51-A43E90F1BD98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -994,7 +991,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10494304" y="754380"/>
+          <a:off x="12799354" y="211455"/>
           <a:ext cx="4155146" cy="3208020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1303,34 +1300,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S196"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q1" sqref="Q1:R1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="Q28" sqref="Q28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="5" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" style="2" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>120</v>
       </c>
@@ -1380,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1430,7 +1427,7 @@
         <v>66.974999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1480,7 +1477,7 @@
         <v>60.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1530,7 +1527,7 @@
         <v>65.05</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1580,7 +1577,7 @@
         <v>60.75</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>59.97</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1680,7 +1677,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1730,7 +1727,7 @@
         <v>63.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1780,7 +1777,7 @@
         <v>59.349999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -1830,7 +1827,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1880,7 +1877,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1930,7 +1927,7 @@
         <v>54.2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1980,7 +1977,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -2030,7 +2027,7 @@
         <v>66.949999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -2080,7 +2077,7 @@
         <v>66.95</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2130,7 +2127,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2230,7 +2227,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -2280,7 +2277,7 @@
         <v>65.849999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2330,7 +2327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2380,7 +2377,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2430,7 +2427,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -2480,7 +2477,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2530,7 +2527,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2580,7 +2577,7 @@
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2630,7 +2627,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2680,7 +2677,7 @@
         <v>69.75</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2730,7 +2727,7 @@
         <v>47.25</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -2780,7 +2777,7 @@
         <v>51.099999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2830,7 +2827,7 @@
         <v>56.55</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2880,7 +2877,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -2930,7 +2927,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -2980,7 +2977,7 @@
         <v>30.799999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -3030,7 +3027,7 @@
         <v>35.849999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -3080,7 +3077,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3130,7 +3127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -3177,7 +3174,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3</v>
       </c>
@@ -3224,7 +3221,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -3274,7 +3271,7 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -3321,7 +3318,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -3371,7 +3368,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3421,7 +3418,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -3471,7 +3468,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
@@ -3521,7 +3518,7 @@
         <v>69.55</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4</v>
       </c>
@@ -3571,7 +3568,7 @@
         <v>69.650000000000006</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3621,7 +3618,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -3671,7 +3668,7 @@
         <v>66.449999999999989</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3</v>
       </c>
@@ -3721,7 +3718,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
@@ -3771,7 +3768,7 @@
         <v>74.45</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -3821,7 +3818,7 @@
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -3871,7 +3868,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -3921,7 +3918,7 @@
         <v>72.650000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4</v>
       </c>
@@ -3971,7 +3968,7 @@
         <v>77.05</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -4021,7 +4018,7 @@
         <v>72.150000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1</v>
       </c>
@@ -4071,7 +4068,7 @@
         <v>83.55</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -4121,7 +4118,7 @@
         <v>79.2</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -4171,7 +4168,7 @@
         <v>77.949999999999989</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4</v>
       </c>
@@ -4221,7 +4218,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -4271,7 +4268,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -4321,7 +4318,7 @@
         <v>69.75</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4</v>
       </c>
@@ -4371,7 +4368,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
@@ -4421,7 +4418,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4</v>
       </c>
@@ -4471,7 +4468,7 @@
         <v>67.949999999999989</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -4521,7 +4518,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
@@ -4571,7 +4568,7 @@
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1</v>
       </c>
@@ -4621,7 +4618,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1</v>
       </c>
@@ -4671,7 +4668,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -4721,7 +4718,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2</v>
       </c>
@@ -4771,7 +4768,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -4821,7 +4818,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1</v>
       </c>
@@ -4871,7 +4868,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2</v>
       </c>
@@ -4921,7 +4918,7 @@
         <v>27.25</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4</v>
       </c>
@@ -4971,7 +4968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
@@ -5021,7 +5018,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -5071,7 +5068,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1</v>
       </c>
@@ -5118,7 +5115,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2</v>
       </c>
@@ -5168,7 +5165,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>3</v>
       </c>
@@ -5218,7 +5215,7 @@
         <v>25.299999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -5268,7 +5265,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
@@ -5318,7 +5315,7 @@
         <v>27.85</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2</v>
       </c>
@@ -5368,7 +5365,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>3</v>
       </c>
@@ -5418,7 +5415,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -5468,7 +5465,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1</v>
       </c>
@@ -5518,7 +5515,7 @@
         <v>71.95</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2</v>
       </c>
@@ -5568,7 +5565,7 @@
         <v>65.699999999999989</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3</v>
       </c>
@@ -5618,7 +5615,7 @@
         <v>66.05</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -5668,7 +5665,7 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1</v>
       </c>
@@ -5718,7 +5715,7 @@
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -5768,7 +5765,7 @@
         <v>71.95</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3</v>
       </c>
@@ -5818,7 +5815,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -5868,7 +5865,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>122</v>
       </c>
@@ -5912,7 +5909,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>122</v>
       </c>
@@ -5956,7 +5953,7 @@
         <v>56.75</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>122</v>
       </c>
@@ -6000,7 +5997,7 @@
         <v>56.15</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>122</v>
       </c>
@@ -6044,7 +6041,7 @@
         <v>104.85</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>122</v>
       </c>
@@ -6088,7 +6085,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>122</v>
       </c>
@@ -6132,7 +6129,7 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>122</v>
       </c>
@@ -6176,7 +6173,7 @@
         <v>53.65</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>122</v>
       </c>
@@ -6220,7 +6217,7 @@
         <v>42.95</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>122</v>
       </c>
@@ -6264,7 +6261,7 @@
         <v>33.450000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>122</v>
       </c>
@@ -6308,7 +6305,7 @@
         <v>27.75</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1</v>
       </c>
@@ -6358,7 +6355,7 @@
         <v>73.949999999999989</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
@@ -6408,7 +6405,7 @@
         <v>70.05</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
@@ -6458,7 +6455,7 @@
         <v>63.75</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1</v>
       </c>
@@ -6508,7 +6505,7 @@
         <v>61.85</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
@@ -6558,7 +6555,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1</v>
       </c>
@@ -6608,7 +6605,7 @@
         <v>47.05</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
@@ -6658,7 +6655,7 @@
         <v>41.95</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1</v>
       </c>
@@ -6708,7 +6705,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1</v>
       </c>
@@ -6758,7 +6755,7 @@
         <v>39.849999999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>4</v>
       </c>
@@ -6808,7 +6805,7 @@
         <v>71.75</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>67</v>
       </c>
@@ -6852,7 +6849,7 @@
         <v>122.95</v>
       </c>
     </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>67</v>
       </c>
@@ -6896,7 +6893,7 @@
         <v>118.25</v>
       </c>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>67</v>
       </c>
@@ -6940,7 +6937,7 @@
         <v>108.1</v>
       </c>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>67</v>
       </c>
@@ -6984,7 +6981,7 @@
         <v>98.050000000000011</v>
       </c>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>67</v>
       </c>
@@ -7028,7 +7025,7 @@
         <v>81.349999999999994</v>
       </c>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>67</v>
       </c>
@@ -7072,7 +7069,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>67</v>
       </c>
@@ -7116,7 +7113,7 @@
         <v>47.099999999999994</v>
       </c>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>67</v>
       </c>
@@ -7160,7 +7157,7 @@
         <v>76.849999999999994</v>
       </c>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>67</v>
       </c>
@@ -7204,7 +7201,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>67</v>
       </c>
@@ -7248,7 +7245,7 @@
         <v>65.95</v>
       </c>
     </row>
-    <row r="122" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>67</v>
       </c>
@@ -7292,7 +7289,7 @@
         <v>67.55</v>
       </c>
     </row>
-    <row r="123" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>67</v>
       </c>
@@ -7336,7 +7333,7 @@
         <v>65.800000000000011</v>
       </c>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>67</v>
       </c>
@@ -7380,7 +7377,7 @@
         <v>65.800000000000011</v>
       </c>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>110</v>
       </c>
@@ -7424,7 +7421,7 @@
         <v>92.1</v>
       </c>
     </row>
-    <row r="126" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>110</v>
       </c>
@@ -7466,7 +7463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="127" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>67</v>
       </c>
@@ -7510,7 +7507,7 @@
         <v>29.75</v>
       </c>
     </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>67</v>
       </c>
@@ -7552,7 +7549,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="129" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>67</v>
       </c>
@@ -7594,7 +7591,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>67</v>
       </c>
@@ -7638,7 +7635,7 @@
         <v>18.350000000000001</v>
       </c>
     </row>
-    <row r="131" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>67</v>
       </c>
@@ -7682,7 +7679,7 @@
         <v>27.5</v>
       </c>
     </row>
-    <row r="132" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>67</v>
       </c>
@@ -7726,7 +7723,7 @@
         <v>54.1</v>
       </c>
     </row>
-    <row r="133" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>67</v>
       </c>
@@ -7767,7 +7764,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>67</v>
       </c>
@@ -7808,7 +7805,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="135" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>67</v>
       </c>
@@ -7849,7 +7846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>122</v>
       </c>
@@ -7893,7 +7890,7 @@
         <v>81.55</v>
       </c>
     </row>
-    <row r="137" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>122</v>
       </c>
@@ -7937,7 +7934,7 @@
         <v>84.7</v>
       </c>
     </row>
-    <row r="138" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>122</v>
       </c>
@@ -7981,7 +7978,7 @@
         <v>86.4</v>
       </c>
     </row>
-    <row r="139" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>122</v>
       </c>
@@ -8025,7 +8022,7 @@
         <v>81.550000000000011</v>
       </c>
     </row>
-    <row r="140" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>122</v>
       </c>
@@ -8069,7 +8066,7 @@
         <v>105.5</v>
       </c>
     </row>
-    <row r="141" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>122</v>
       </c>
@@ -8113,7 +8110,7 @@
         <v>83.95</v>
       </c>
     </row>
-    <row r="142" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B142" t="s">
         <v>122</v>
       </c>
@@ -8157,7 +8154,7 @@
         <v>91.6</v>
       </c>
     </row>
-    <row r="143" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B143" t="s">
         <v>122</v>
       </c>
@@ -8201,7 +8198,7 @@
         <v>99.3</v>
       </c>
     </row>
-    <row r="144" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B144" t="s">
         <v>122</v>
       </c>
@@ -8246,7 +8243,7 @@
       </c>
       <c r="S144" s="3"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" t="s">
         <v>122</v>
       </c>
@@ -8290,7 +8287,7 @@
         <v>105.55000000000001</v>
       </c>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
         <v>122</v>
       </c>
@@ -8334,7 +8331,7 @@
         <v>100.5</v>
       </c>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" t="s">
         <v>122</v>
       </c>
@@ -8378,7 +8375,7 @@
         <v>103.05000000000001</v>
       </c>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" t="s">
         <v>122</v>
       </c>
@@ -8422,7 +8419,7 @@
         <v>95.65</v>
       </c>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
         <v>122</v>
       </c>
@@ -8466,7 +8463,7 @@
         <v>85.15</v>
       </c>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" t="s">
         <v>122</v>
       </c>
@@ -8510,7 +8507,7 @@
         <v>95.1</v>
       </c>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" t="s">
         <v>122</v>
       </c>
@@ -8554,7 +8551,7 @@
         <v>100.85</v>
       </c>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
         <v>122</v>
       </c>
@@ -8598,7 +8595,7 @@
         <v>88.35</v>
       </c>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" t="s">
         <v>122</v>
       </c>
@@ -8642,7 +8639,7 @@
         <v>95.550000000000011</v>
       </c>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" t="s">
         <v>122</v>
       </c>
@@ -8686,7 +8683,7 @@
         <v>89.6</v>
       </c>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" t="s">
         <v>122</v>
       </c>
@@ -8730,7 +8727,7 @@
         <v>83.800000000000011</v>
       </c>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" t="s">
         <v>122</v>
       </c>
@@ -8774,7 +8771,7 @@
         <v>68.25</v>
       </c>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" t="s">
         <v>122</v>
       </c>
@@ -8818,7 +8815,7 @@
         <v>89.449999999999989</v>
       </c>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" t="s">
         <v>122</v>
       </c>
@@ -8862,7 +8859,7 @@
         <v>82.4</v>
       </c>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
         <v>122</v>
       </c>
@@ -8906,7 +8903,7 @@
         <v>70.199999999999989</v>
       </c>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" t="s">
         <v>122</v>
       </c>
@@ -8950,7 +8947,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B161" t="s">
         <v>122</v>
       </c>
@@ -8994,7 +8991,7 @@
         <v>88.35</v>
       </c>
     </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
         <v>122</v>
       </c>
@@ -9038,7 +9035,7 @@
         <v>78.25</v>
       </c>
     </row>
-    <row r="163" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B163" t="s">
         <v>122</v>
       </c>
@@ -9082,7 +9079,7 @@
         <v>82.199999999999989</v>
       </c>
     </row>
-    <row r="164" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
         <v>122</v>
       </c>
@@ -9126,7 +9123,7 @@
         <v>87.75</v>
       </c>
     </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B165" t="s">
         <v>122</v>
       </c>
@@ -9170,7 +9167,7 @@
         <v>80.349999999999994</v>
       </c>
     </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B166" t="s">
         <v>122</v>
       </c>
@@ -9214,7 +9211,7 @@
         <v>91.699999999999989</v>
       </c>
     </row>
-    <row r="167" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>122</v>
       </c>
@@ -9258,7 +9255,7 @@
         <v>81.45</v>
       </c>
     </row>
-    <row r="168" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
         <v>122</v>
       </c>
@@ -9302,7 +9299,7 @@
         <v>79.150000000000006</v>
       </c>
     </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B169" t="s">
         <v>122</v>
       </c>
@@ -9346,7 +9343,7 @@
         <v>85.05</v>
       </c>
     </row>
-    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B170" t="s">
         <v>122</v>
       </c>
@@ -9390,7 +9387,7 @@
         <v>83.35</v>
       </c>
     </row>
-    <row r="171" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
         <v>122</v>
       </c>
@@ -9434,7 +9431,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B172" t="s">
         <v>122</v>
       </c>
@@ -9478,7 +9475,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="173" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B173" t="s">
         <v>122</v>
       </c>
@@ -9522,7 +9519,7 @@
         <v>17.5</v>
       </c>
     </row>
-    <row r="174" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B174" t="s">
         <v>122</v>
       </c>
@@ -9566,7 +9563,7 @@
         <v>15.899999999999999</v>
       </c>
     </row>
-    <row r="175" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B175" t="s">
         <v>122</v>
       </c>
@@ -9610,7 +9607,7 @@
         <v>20.45</v>
       </c>
     </row>
-    <row r="176" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B176" t="s">
         <v>122</v>
       </c>
@@ -9654,7 +9651,7 @@
         <v>16.100000000000001</v>
       </c>
     </row>
-    <row r="177" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B177" t="s">
         <v>122</v>
       </c>
@@ -9698,7 +9695,7 @@
         <v>17.600000000000001</v>
       </c>
     </row>
-    <row r="178" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
         <v>122</v>
       </c>
@@ -9742,7 +9739,7 @@
         <v>90.949999999999989</v>
       </c>
     </row>
-    <row r="179" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B179" t="s">
         <v>122</v>
       </c>
@@ -9786,7 +9783,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="180" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B180" t="s">
         <v>122</v>
       </c>
@@ -9830,7 +9827,7 @@
         <v>84.4</v>
       </c>
     </row>
-    <row r="181" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B181" t="s">
         <v>122</v>
       </c>
@@ -9874,7 +9871,7 @@
         <v>80.849999999999994</v>
       </c>
     </row>
-    <row r="182" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B182" t="s">
         <v>122</v>
       </c>
@@ -9918,7 +9915,7 @@
         <v>83.75</v>
       </c>
     </row>
-    <row r="183" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B183" t="s">
         <v>122</v>
       </c>
@@ -9962,7 +9959,7 @@
         <v>85.4</v>
       </c>
     </row>
-    <row r="184" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B184" t="s">
         <v>122</v>
       </c>
@@ -10006,7 +10003,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="185" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B185" t="s">
         <v>122</v>
       </c>
@@ -10050,7 +10047,7 @@
         <v>71.849999999999994</v>
       </c>
     </row>
-    <row r="186" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B186" t="s">
         <v>122</v>
       </c>
@@ -10094,7 +10091,7 @@
         <v>90.15</v>
       </c>
     </row>
-    <row r="187" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B187" t="s">
         <v>122</v>
       </c>
@@ -10138,7 +10135,7 @@
         <v>73.7</v>
       </c>
     </row>
-    <row r="188" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B188" t="s">
         <v>122</v>
       </c>
@@ -10183,7 +10180,7 @@
       </c>
       <c r="S188" s="3"/>
     </row>
-    <row r="189" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B189" t="s">
         <v>122</v>
       </c>
@@ -10227,7 +10224,7 @@
         <v>88.25</v>
       </c>
     </row>
-    <row r="190" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B190" t="s">
         <v>122</v>
       </c>
@@ -10271,7 +10268,7 @@
         <v>73.599999999999994</v>
       </c>
     </row>
-    <row r="191" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
         <v>122</v>
       </c>
@@ -10315,7 +10312,7 @@
         <v>77.8</v>
       </c>
     </row>
-    <row r="192" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B192" t="s">
         <v>122</v>
       </c>
@@ -10359,7 +10356,7 @@
         <v>82.3</v>
       </c>
     </row>
-    <row r="193" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
         <v>122</v>
       </c>
@@ -10403,7 +10400,7 @@
         <v>83.25</v>
       </c>
     </row>
-    <row r="194" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
         <v>122</v>
       </c>
@@ -10447,7 +10444,7 @@
         <v>99.8</v>
       </c>
     </row>
-    <row r="195" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B195" t="s">
         <v>122</v>
       </c>
@@ -10491,7 +10488,7 @@
         <v>80.599999999999994</v>
       </c>
     </row>
-    <row r="196" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
         <v>122</v>
       </c>
@@ -10536,6 +10533,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P196" xr:uid="{9D0DA90A-6ADF-4546-9FD5-3306B2ABDFA9}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -10544,16 +10542,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O126"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C91" sqref="C91"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10600,7 +10598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10647,7 +10645,7 @@
         <v>66.974999999999994</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10694,7 +10692,7 @@
         <v>60.900000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10741,7 +10739,7 @@
         <v>65.05</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10788,7 +10786,7 @@
         <v>60.75</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -10835,7 +10833,7 @@
         <v>59.97</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -10882,7 +10880,7 @@
         <v>63.4</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2</v>
       </c>
@@ -10929,7 +10927,7 @@
         <v>63.400000000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>3</v>
       </c>
@@ -10976,7 +10974,7 @@
         <v>59.349999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>4</v>
       </c>
@@ -11023,7 +11021,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
@@ -11070,7 +11068,7 @@
         <v>60.3</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -11117,7 +11115,7 @@
         <v>54.2</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -11164,7 +11162,7 @@
         <v>64.3</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>3</v>
       </c>
@@ -11211,7 +11209,7 @@
         <v>66.949999999999989</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>4</v>
       </c>
@@ -11258,7 +11256,7 @@
         <v>66.95</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1</v>
       </c>
@@ -11305,7 +11303,7 @@
         <v>57.7</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -11352,7 +11350,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
@@ -11399,7 +11397,7 @@
         <v>63.2</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
@@ -11446,7 +11444,7 @@
         <v>65.849999999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
@@ -11493,7 +11491,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -11540,7 +11538,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -11587,7 +11585,7 @@
         <v>71.5</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
@@ -11634,7 +11632,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>1</v>
       </c>
@@ -11681,7 +11679,7 @@
         <v>64.400000000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -11728,7 +11726,7 @@
         <v>68.099999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -11775,7 +11773,7 @@
         <v>70.900000000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>4</v>
       </c>
@@ -11822,7 +11820,7 @@
         <v>69.75</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>1</v>
       </c>
@@ -11869,7 +11867,7 @@
         <v>47.25</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>2</v>
       </c>
@@ -11916,7 +11914,7 @@
         <v>51.099999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -11963,7 +11961,7 @@
         <v>56.55</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>4</v>
       </c>
@@ -12010,7 +12008,7 @@
         <v>60.8</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>1</v>
       </c>
@@ -12057,7 +12055,7 @@
         <v>39.4</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>2</v>
       </c>
@@ -12104,7 +12102,7 @@
         <v>30.799999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>3</v>
       </c>
@@ -12151,7 +12149,7 @@
         <v>35.849999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -12198,7 +12196,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>1</v>
       </c>
@@ -12245,7 +12243,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>2</v>
       </c>
@@ -12289,7 +12287,7 @@
         <v>22.7</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>3</v>
       </c>
@@ -12333,7 +12331,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>3</v>
       </c>
@@ -12380,7 +12378,7 @@
         <v>29.35</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -12424,7 +12422,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -12471,7 +12469,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>1</v>
       </c>
@@ -12518,7 +12516,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2</v>
       </c>
@@ -12565,7 +12563,7 @@
         <v>71.599999999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>3</v>
       </c>
@@ -12612,7 +12610,7 @@
         <v>69.55</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>4</v>
       </c>
@@ -12659,7 +12657,7 @@
         <v>69.650000000000006</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>1</v>
       </c>
@@ -12706,7 +12704,7 @@
         <v>61.3</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>2</v>
       </c>
@@ -12753,7 +12751,7 @@
         <v>66.449999999999989</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>3</v>
       </c>
@@ -12800,7 +12798,7 @@
         <v>69.5</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>4</v>
       </c>
@@ -12847,7 +12845,7 @@
         <v>74.45</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>1</v>
       </c>
@@ -12894,7 +12892,7 @@
         <v>72.400000000000006</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>2</v>
       </c>
@@ -12941,7 +12939,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>3</v>
       </c>
@@ -12988,7 +12986,7 @@
         <v>72.650000000000006</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>4</v>
       </c>
@@ -13035,7 +13033,7 @@
         <v>77.05</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>1</v>
       </c>
@@ -13082,7 +13080,7 @@
         <v>72.150000000000006</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>1</v>
       </c>
@@ -13129,7 +13127,7 @@
         <v>83.55</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>2</v>
       </c>
@@ -13176,7 +13174,7 @@
         <v>79.2</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>3</v>
       </c>
@@ -13223,7 +13221,7 @@
         <v>77.949999999999989</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>4</v>
       </c>
@@ -13270,7 +13268,7 @@
         <v>61.2</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>1</v>
       </c>
@@ -13317,7 +13315,7 @@
         <v>60.95</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>2</v>
       </c>
@@ -13364,7 +13362,7 @@
         <v>69.75</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>4</v>
       </c>
@@ -13411,7 +13409,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>4</v>
       </c>
@@ -13458,7 +13456,7 @@
         <v>64.2</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>4</v>
       </c>
@@ -13505,7 +13503,7 @@
         <v>67.949999999999989</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>3</v>
       </c>
@@ -13552,7 +13550,7 @@
         <v>67.099999999999994</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2</v>
       </c>
@@ -13599,7 +13597,7 @@
         <v>68.150000000000006</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>1</v>
       </c>
@@ -13646,7 +13644,7 @@
         <v>62.2</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>1</v>
       </c>
@@ -13693,7 +13691,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>3</v>
       </c>
@@ -13740,7 +13738,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>2</v>
       </c>
@@ -13787,7 +13785,7 @@
         <v>24.6</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>1</v>
       </c>
@@ -13834,7 +13832,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>1</v>
       </c>
@@ -13881,7 +13879,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>2</v>
       </c>
@@ -13928,7 +13926,7 @@
         <v>27.25</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>4</v>
       </c>
@@ -13975,7 +13973,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>4</v>
       </c>
@@ -14022,7 +14020,7 @@
         <v>26.25</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>1</v>
       </c>
@@ -14069,7 +14067,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>1</v>
       </c>
@@ -14113,7 +14111,7 @@
         <v>15.5</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>2</v>
       </c>
@@ -14160,7 +14158,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>3</v>
       </c>
@@ -14207,7 +14205,7 @@
         <v>25.299999999999997</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>4</v>
       </c>
@@ -14254,7 +14252,7 @@
         <v>21.85</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>1</v>
       </c>
@@ -14301,7 +14299,7 @@
         <v>27.85</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>2</v>
       </c>
@@ -14348,7 +14346,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>3</v>
       </c>
@@ -14395,7 +14393,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>4</v>
       </c>
@@ -14442,7 +14440,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>1</v>
       </c>
@@ -14489,7 +14487,7 @@
         <v>71.95</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>2</v>
       </c>
@@ -14536,7 +14534,7 @@
         <v>65.699999999999989</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>3</v>
       </c>
@@ -14583,7 +14581,7 @@
         <v>66.05</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>4</v>
       </c>
@@ -14630,7 +14628,7 @@
         <v>61.4</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>1</v>
       </c>
@@ -14677,7 +14675,7 @@
         <v>74.150000000000006</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2</v>
       </c>
@@ -14724,7 +14722,7 @@
         <v>71.95</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>3</v>
       </c>
@@ -14771,7 +14769,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>4</v>
       </c>
@@ -14818,7 +14816,7 @@
         <v>70.2</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>110</v>
       </c>
@@ -14859,7 +14857,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>110</v>
       </c>
@@ -14900,7 +14898,7 @@
         <v>56.75</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>110</v>
       </c>
@@ -14941,7 +14939,7 @@
         <v>56.15</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>110</v>
       </c>
@@ -14982,7 +14980,7 @@
         <v>104.85</v>
       </c>
     </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>110</v>
       </c>
@@ -15023,7 +15021,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>110</v>
       </c>
@@ -15064,7 +15062,7 @@
         <v>65.900000000000006</v>
       </c>
     </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>110</v>
       </c>
@@ -15105,7 +15103,7 @@
         <v>53.65</v>
       </c>
     </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>110</v>
       </c>
@@ -15146,7 +15144,7 @@
         <v>42.95</v>
       </c>
     </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>110</v>
       </c>
@@ -15187,7 +15185,7 @@
         <v>33.450000000000003</v>
       </c>
     </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>110</v>
       </c>
@@ -15228,7 +15226,7 @@
         <v>27.75</v>
       </c>
     </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>1</v>
       </c>
@@ -15275,7 +15273,7 @@
         <v>73.949999999999989</v>
       </c>
     </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>1</v>
       </c>
@@ -15322,7 +15320,7 @@
         <v>70.05</v>
       </c>
     </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>1</v>
       </c>
@@ -15369,7 +15367,7 @@
         <v>63.75</v>
       </c>
     </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>1</v>
       </c>
@@ -15416,7 +15414,7 @@
         <v>61.85</v>
       </c>
     </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>1</v>
       </c>
@@ -15463,7 +15461,7 @@
         <v>53.2</v>
       </c>
     </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>1</v>
       </c>
@@ -15510,7 +15508,7 @@
         <v>47.05</v>
       </c>
     </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>1</v>
       </c>
@@ -15557,7 +15555,7 @@
         <v>41.95</v>
       </c>
     </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>1</v>
       </c>
@@ -15604,7 +15602,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>1</v>
       </c>
@@ -15651,7 +15649,7 @@
         <v>39.849999999999994</v>
       </c>
     </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>4</v>
       </c>
@@ -15698,7 +15696,7 @@
         <v>71.75</v>
       </c>
     </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>67</v>
       </c>
@@ -15739,7 +15737,7 @@
         <v>122.95</v>
       </c>
     </row>
-    <row r="113" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>67</v>
       </c>
@@ -15781,7 +15779,7 @@
         <v>118.25</v>
       </c>
     </row>
-    <row r="114" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>67</v>
       </c>
@@ -15822,7 +15820,7 @@
         <v>108.1</v>
       </c>
     </row>
-    <row r="115" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>67</v>
       </c>
@@ -15863,7 +15861,7 @@
         <v>98.050000000000011</v>
       </c>
     </row>
-    <row r="116" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>67</v>
       </c>
@@ -15904,7 +15902,7 @@
         <v>81.349999999999994</v>
       </c>
     </row>
-    <row r="117" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>67</v>
       </c>
@@ -15945,7 +15943,7 @@
         <v>71.400000000000006</v>
       </c>
     </row>
-    <row r="118" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>67</v>
       </c>
@@ -15986,7 +15984,7 @@
         <v>47.099999999999994</v>
       </c>
     </row>
-    <row r="119" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>67</v>
       </c>
@@ -16027,7 +16025,7 @@
         <v>76.8</v>
       </c>
     </row>
-    <row r="120" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>67</v>
       </c>
@@ -16068,7 +16066,7 @@
         <v>65.7</v>
       </c>
     </row>
-    <row r="121" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>67</v>
       </c>
@@ -16109,7 +16107,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="122" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>67</v>
       </c>
@@ -16150,7 +16148,7 @@
         <v>67.599999999999994</v>
       </c>
     </row>
-    <row r="123" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>67</v>
       </c>
@@ -16191,7 +16189,7 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="124" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>67</v>
       </c>
@@ -16232,7 +16230,7 @@
         <v>65.8</v>
       </c>
     </row>
-    <row r="125" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>67</v>
       </c>
@@ -16251,8 +16249,9 @@
       <c r="H125" t="s">
         <v>42</v>
       </c>
-      <c r="I125" t="s">
-        <v>119</v>
+      <c r="I125">
+        <f>B431</f>
+        <v>0</v>
       </c>
       <c r="J125" t="s">
         <v>29</v>
@@ -16274,7 +16273,7 @@
         <v>92.1</v>
       </c>
     </row>
-    <row r="126" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>67</v>
       </c>

</xml_diff>